<commit_message>
Modify the BOM table and add frame0.step
Signed-off-by: XG. <857439011@qq.com>
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="63">
   <si>
     <t>序号</t>
   </si>
@@ -124,97 +124,100 @@
     <t>圆锥滚子轴承</t>
   </si>
   <si>
+    <t>20*37*12</t>
+  </si>
+  <si>
+    <t>https://detail.tmall.com/item.htm?id=616787169746&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.66912e8dUnU3HP&amp;pisk=g2Dgsk6FFfP6eYYL9vw6aaGV4uAL-Rwj3qBYk-U2TyzBc1C9fSrqmqDx6mzYnq0moPF25RHm-0ivfxK_QKqqy22xXPUx-n0tctL6GRBVoViy5cUvfx44-Vu0GhaYur0x0fKpeLnsf-w4nUpJerVXm80GgOrw09r_4HEwAfJqa-w2yEfd359uhVyAlb1NTkzQmo740qyUToq43ora3H4Umu1V7qu2xyr8qs54_r5eLyZ8bsWN3wyUqlbN3ou48HqY8ry4_qoEiRW4rxkILeILHtKsngN3j54rbPoTBv5Qv1Ma-R2sIlmHxc43vkH3j54zOQgvBAuK0AH_OQC7hDhoojueKO0mbbu4Wv8PnrhSCDk3ZiWxxJ4mVPyl0do3IPVrpV9PH4on0bFnp3J7IRzZMRiAqFnnIVnsKmIVTR2tt7DgUL_akXnonoDXlp0obbuqigyNT_r05tZeDv5fG5rQxzCEBz-Xhtj4EHxhNCNaAlLJxHffG5rQxzKHx____kZ9y</t>
+  </si>
+  <si>
+    <t>十字扁平头螺丝</t>
+  </si>
+  <si>
+    <t>M3*8</t>
+  </si>
+  <si>
+    <t>https://detail.tmall.com/item.htm?id=641493636015&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.66912e8dUnU3HP&amp;pisk=g0L8smfSGxDuTJ8RiQo0K7BtZlhDRmAygLR_-9XuAKpvpCFkqMXhAwpwBMan4ajdJK6DrTAlP6sBKdtlF3X3Jep2ez4hPp0ddC-qTTfkrWCBcLUHqQXkDWQyo34hEY7pOdbKIA0iSQRPuwMiIYohfz71s9ZQK_1flwfpmQZu1QRP89N0dcxXaWp22_F5O9GAl6C7Aws5OZNf36q5dp65c-1O_w_BdTabl1CGNy1QVjEf_6UQNT1Cho1F9u_CVpOjM6WfNw_IMbHdh763JhDl0vlnfrmsfECR29UHbyBMIPXCCiB0RAwdNgEkNtUQREKmLVmCFcPcLaXyt_pE7z75v39RGw3LlapyNesv-xVfXZ6dfUjY1rsDe6I1RiFQRIQ20p1c5VwAgnOkAUJ89y1yrFjdQihQ8MbXSGt6eWlwGa1BLG8nQzWWOC8wjN3LlaIC4KYMW42aIOC3VjhYYkS5gnGBnZAbvlIfMOc-JkrF0j5AIjhYYkS5gsBiwXEUYilV.</t>
+  </si>
+  <si>
+    <t>内六角螺丝圆柱头螺栓</t>
+  </si>
+  <si>
+    <t>M5*14</t>
+  </si>
+  <si>
+    <t>https://detail.tmall.com/item.htm?id=40189700729&amp;pisk=gJG_s6cDkGj6j-PAlRYFOvo2Z7Vb5eRyMZaxrqCNk5FThs3ZVr543d4fGkgJSlJDImMIDD2aXoy4GrizxV52SV8XGq38XSkabrnEcDXZbjrqYIgoVR5Zkj7iK0uR_fJggsNgiSKy4QRr7VV0MGdi8PsgJzU6grETD5Vd4l_weQRrS2_aWUupaj8X6P41HsnYBJQLrkUTkOU9RJUzkSCTH1BdvkqLMreYMyBLkr6OHRnYJ2U4WNITMSILpPrLDSFxD2LQlkExMxvQJdZE5Fr6zQUBBBM3AsCxOyt08V_1dol45YqSWVvkEE4_Cu3TAhCJWBwKo-GcoswZWYm0ycI9fS3QP0aSfK70fv3r_x36O3FZsVH8HbKcH0Nsc8hTdZCjS5r3OyhJuTqEOlox1JLPN-PKa8FtLpxa35aSDfm1lsn-84lgKjt5voDarWUsDQKC4zCzVDHGhwwlGyZyRe6cnVt1Ybz4fVUbBy4hzeTCUt2T-yZyRe6cnRU3-Q8BRTWc.&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.66b22e8dWKj7Gf</t>
+  </si>
+  <si>
+    <t>M4*14</t>
+  </si>
+  <si>
+    <t>六角螺帽</t>
+  </si>
+  <si>
+    <t>M5</t>
+  </si>
+  <si>
+    <t>https://detail.tmall.com/item.htm?detail_redpacket_pop=true&amp;id=549640610734&amp;ltk2=1751972028937ji8m1jp7ssaci3uz6zdys&amp;ns=1&amp;priceTId=undefined&amp;query=m5%E8%9E%BA%E6%AF%8D&amp;skuId=5618615008389&amp;spm=a21n57.1.hoverItem.1&amp;utparam=%7B%22aplus_abtest%22%3A%2203691c8cc532103ef1eb26baed91686a%22%7D&amp;xxc=ad_ztc</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>https://detail.tmall.com/item.htm?id=549640610734&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.1e082e8dJs5w32&amp;pisk=gHo3_1w_52zQ_gATWcZBu6qVuZTtRkZS4bI8wuFy75P6FwQpdzyrEbm-JYP8qbcoZWUyOknosxMJd0pQY32rMfq-pWF-sLcKFgdBPkIPZXM2OvFJd0VzsXluPpN8a7c-U2p9DnHIduZzZIKvDc8xORlh8WPyUPy7UdeeC2-ruuZyMQbO4yt0VXrRB9_P7RP_E85zab-a78NaUwrra5za3-CU4blz_AyQn97P8g-aQ5wc49yzaA7ae85FY7lrQd28EuPrayJiQjf2TWorvcROUHSOhzRsYJ43gvPnpAmwlP_Ip5mxVcynPJMFPgSrjJ4nbr7E3Y4KzxajvvKlfkHm7lynanRUbxuiHymHiMF7rccnrXpRPR0oUmZQmT-EIkV3uD4CFicqIYuYScp2ckqUT4EIetAKIDcKdcDRUNr3vV4mxo-fT73tn02oVQtiivuqa4jrjN7VxkS7QLnNPaaUCRVA7DF2FEN299JMIZV78RwUMdvGPaaUCRVvIdbmFyy_LSC..</t>
+  </si>
+  <si>
+    <t>土八热熔螺母</t>
+  </si>
+  <si>
+    <t>M2*2*3</t>
+  </si>
+  <si>
+    <t>https://detail.tmall.com/item.htm?id=809364062256&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.1e082e8dJs5w32&amp;pisk=gXH3sUq_1XPI37LT6AwBgw2VgsOTpJwSU4B8y8Uy_Pz6V6CpA7rrq4D-90z8E40oryFyRJHoSmiJAYKQLLqrkV2-vyU-S30KVTLBNJBPr2i2RDUJAY4zS2uuNHa8zz0-4XK9HKnIA8wzrEpvHARxRluhU9Pe45r8qhEefXJrg8wykUfOUW90F2yRXn5F_lz_qu7zz4Ja_uaa46yrzPPa0oQUU4uz7crQmM5PTTJabPZUzMzU4loamuEPTuurbhq77zyzT4oZi58U8YkKQFIyLOIbEgHYxW4qYymKjA-gw6i_SbhSBkc7GD55UTkgxWDag6oqqWhrcSMKvLX_pmcaQk0y3eyZ0fmYtvYcpzNoI2coJ3C7jbmrhJwc4pogKyVqKWs5nqoi4jFiBnJbKJzEwJiRmeniK2nII0IP_J2KsSD33K_UyfnmEuDWPd0mYjurZg-G_sW3LTZw2A55NWr_jrCZpr-WGr8dYhxGizNUfkzvjhf5NWr_jrKMjsm7TlZUk</t>
+  </si>
+  <si>
+    <t>3M同步轮</t>
+  </si>
+  <si>
+    <t>3M25齿 孔8 宽11</t>
+  </si>
+  <si>
+    <t>https://item.taobao.com/item.htm?spm=tbpc.boughtlist.suborder_itemtitle.1.1e082e8dJs5w32&amp;id=739009813395&amp;pisk=gS4g6qGIAlo6EvXKvyg14d0y43sLXVgbu-LxHqHVYvkCGhKO1ml4i-4YXSkxo-20nAnVCVU0K7NA1rCs7Zc4eJ0Y6AHYKs2TGEB1cVL2nRNPC5HA1rDqKRymc1Mx3x2YglCdyaF_1qgqnTQRyyS8CXrDuFlVgBltofrLbhEz1qgVnBLV2aV_CJRJHhlqT6cxMK843fJELvGvbxyqQDJEZbgqu-kaTBl-snRwuhlFtblX_xu2bBuEgjOwb-uVtWkIgqla3ql0aOkauPUFpI7wJQZholGijYPZI5eL83gkfJM35yaosoZu_nT2uycijyoyb7PmXoPSVPFOoegTZkuEs-7PQ2Pzx7ngSTYthm43Io2OMnG3mSzS54AV7W0iI0zifITuUWV42D4daagi7Arx5SdlBW4gB5a3MI-ESVEnqP0PPdkYv74mir6f-8Va4-rc4Exe4F0wlX5Y8ntjbXGneHztUssSUOdNt6xohclI_YChtntjbXGne6fHqSiZOfkR.</t>
+  </si>
+  <si>
+    <t>3M25齿 孔5 宽11</t>
+  </si>
+  <si>
+    <t>3M25齿 孔6 宽11</t>
+  </si>
+  <si>
+    <t>3M同步带</t>
+  </si>
+  <si>
+    <t>3M-长171-宽11</t>
+  </si>
+  <si>
+    <t>3M-长177-宽11</t>
+  </si>
+  <si>
+    <t>联轴器</t>
+  </si>
+  <si>
+    <t>外径28mm抱紧式联轴器 孔径8mm</t>
+  </si>
+  <si>
+    <t>https://buyertrade.taobao.com/trade/itemlist/list_bought_items.htm?spm=a21bo.jianhua/a.bought.1.5af92a89D0sxQv</t>
+  </si>
+  <si>
+    <t>限位开关</t>
+  </si>
+  <si>
+    <t>KW11-3Z-A</t>
+  </si>
+  <si>
+    <t>https://item.taobao.com/item.htm?spm=tbpc.boughtlist.suborder_itemtitle.1.12492e8dAwCxKM&amp;id=630808292950&amp;pisk=gprTs5D1d6fGaYZtKR7HilnkVyWnBw2aL5yWmjcMlWFLM8pgSqcmlmFzwqtc7c0xDWG3jf2ifxgbi7ai1PcDDoFU6hxmfSjxG8zF3fDgjKHbR5K0SRcgJKnaxPxms1oYh7mAZ_jlqRyZYm1lZXrvVsnSUxM6if9BRmDY-RTMFRyZ0j9HGa4QQKFhug9shj6KAxH6lmMjhJ6KHYhjcfgXOeMSOmiX5FTIdxktGjgbGeGI3AGXGqTsRMMohmT_GVsCpxlICmijMt5xOdGDDzfxdedv5g-pvkHtWjKmPneQq30xNtc90nltsVLgCXKXckUhggbj1aJngccanAFV4hoskPNtdmIvAcFaCogLm6vIyDGxPl0pFHg36x3Sc2pXcJnU8SMnVgOKLywgllP9HnMaju0xa2BX0qmQq4a76KWzdcMbg4rcahl_h8rzr0IvAc3f4Squ2GAyZbHD59BpuEusLy6btD2BkU3IpbXODE8q89kKZ9BpuEusLvhlBtL2u2WF.</t>
+  </si>
+  <si>
     <t>KW11-3Z-B</t>
-  </si>
-  <si>
-    <t>https://detail.tmall.com/item.htm?id=616787169746&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.66912e8dUnU3HP&amp;pisk=g2Dgsk6FFfP6eYYL9vw6aaGV4uAL-Rwj3qBYk-U2TyzBc1C9fSrqmqDx6mzYnq0moPF25RHm-0ivfxK_QKqqy22xXPUx-n0tctL6GRBVoViy5cUvfx44-Vu0GhaYur0x0fKpeLnsf-w4nUpJerVXm80GgOrw09r_4HEwAfJqa-w2yEfd359uhVyAlb1NTkzQmo740qyUToq43ora3H4Umu1V7qu2xyr8qs54_r5eLyZ8bsWN3wyUqlbN3ou48HqY8ry4_qoEiRW4rxkILeILHtKsngN3j54rbPoTBv5Qv1Ma-R2sIlmHxc43vkH3j54zOQgvBAuK0AH_OQC7hDhoojueKO0mbbu4Wv8PnrhSCDk3ZiWxxJ4mVPyl0do3IPVrpV9PH4on0bFnp3J7IRzZMRiAqFnnIVnsKmIVTR2tt7DgUL_akXnonoDXlp0obbuqigyNT_r05tZeDv5fG5rQxzCEBz-Xhtj4EHxhNCNaAlLJxHffG5rQxzKHx____kZ9y</t>
-  </si>
-  <si>
-    <t>十字扁平头螺丝</t>
-  </si>
-  <si>
-    <t>M3*8</t>
-  </si>
-  <si>
-    <t>https://detail.tmall.com/item.htm?id=641493636015&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.66912e8dUnU3HP&amp;pisk=g0L8smfSGxDuTJ8RiQo0K7BtZlhDRmAygLR_-9XuAKpvpCFkqMXhAwpwBMan4ajdJK6DrTAlP6sBKdtlF3X3Jep2ez4hPp0ddC-qTTfkrWCBcLUHqQXkDWQyo34hEY7pOdbKIA0iSQRPuwMiIYohfz71s9ZQK_1flwfpmQZu1QRP89N0dcxXaWp22_F5O9GAl6C7Aws5OZNf36q5dp65c-1O_w_BdTabl1CGNy1QVjEf_6UQNT1Cho1F9u_CVpOjM6WfNw_IMbHdh763JhDl0vlnfrmsfECR29UHbyBMIPXCCiB0RAwdNgEkNtUQREKmLVmCFcPcLaXyt_pE7z75v39RGw3LlapyNesv-xVfXZ6dfUjY1rsDe6I1RiFQRIQ20p1c5VwAgnOkAUJ89y1yrFjdQihQ8MbXSGt6eWlwGa1BLG8nQzWWOC8wjN3LlaIC4KYMW42aIOC3VjhYYkS5gnGBnZAbvlIfMOc-JkrF0j5AIjhYYkS5gsBiwXEUYilV.</t>
-  </si>
-  <si>
-    <t>内六角螺丝圆柱头螺栓</t>
-  </si>
-  <si>
-    <t>M5*14</t>
-  </si>
-  <si>
-    <t>https://detail.tmall.com/item.htm?id=40189700729&amp;pisk=gJG_s6cDkGj6j-PAlRYFOvo2Z7Vb5eRyMZaxrqCNk5FThs3ZVr543d4fGkgJSlJDImMIDD2aXoy4GrizxV52SV8XGq38XSkabrnEcDXZbjrqYIgoVR5Zkj7iK0uR_fJggsNgiSKy4QRr7VV0MGdi8PsgJzU6grETD5Vd4l_weQRrS2_aWUupaj8X6P41HsnYBJQLrkUTkOU9RJUzkSCTH1BdvkqLMreYMyBLkr6OHRnYJ2U4WNITMSILpPrLDSFxD2LQlkExMxvQJdZE5Fr6zQUBBBM3AsCxOyt08V_1dol45YqSWVvkEE4_Cu3TAhCJWBwKo-GcoswZWYm0ycI9fS3QP0aSfK70fv3r_x36O3FZsVH8HbKcH0Nsc8hTdZCjS5r3OyhJuTqEOlox1JLPN-PKa8FtLpxa35aSDfm1lsn-84lgKjt5voDarWUsDQKC4zCzVDHGhwwlGyZyRe6cnVt1Ybz4fVUbBy4hzeTCUt2T-yZyRe6cnRU3-Q8BRTWc.&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.66b22e8dWKj7Gf</t>
-  </si>
-  <si>
-    <t>M4*14</t>
-  </si>
-  <si>
-    <t>六角螺帽</t>
-  </si>
-  <si>
-    <t>M5</t>
-  </si>
-  <si>
-    <t>https://detail.tmall.com/item.htm?detail_redpacket_pop=true&amp;id=549640610734&amp;ltk2=1751972028937ji8m1jp7ssaci3uz6zdys&amp;ns=1&amp;priceTId=undefined&amp;query=m5%E8%9E%BA%E6%AF%8D&amp;skuId=5618615008389&amp;spm=a21n57.1.hoverItem.1&amp;utparam=%7B%22aplus_abtest%22%3A%2203691c8cc532103ef1eb26baed91686a%22%7D&amp;xxc=ad_ztc</t>
-  </si>
-  <si>
-    <t>M3</t>
-  </si>
-  <si>
-    <t>https://detail.tmall.com/item.htm?id=549640610734&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.1e082e8dJs5w32&amp;pisk=gHo3_1w_52zQ_gATWcZBu6qVuZTtRkZS4bI8wuFy75P6FwQpdzyrEbm-JYP8qbcoZWUyOknosxMJd0pQY32rMfq-pWF-sLcKFgdBPkIPZXM2OvFJd0VzsXluPpN8a7c-U2p9DnHIduZzZIKvDc8xORlh8WPyUPy7UdeeC2-ruuZyMQbO4yt0VXrRB9_P7RP_E85zab-a78NaUwrra5za3-CU4blz_AyQn97P8g-aQ5wc49yzaA7ae85FY7lrQd28EuPrayJiQjf2TWorvcROUHSOhzRsYJ43gvPnpAmwlP_Ip5mxVcynPJMFPgSrjJ4nbr7E3Y4KzxajvvKlfkHm7lynanRUbxuiHymHiMF7rccnrXpRPR0oUmZQmT-EIkV3uD4CFicqIYuYScp2ckqUT4EIetAKIDcKdcDRUNr3vV4mxo-fT73tn02oVQtiivuqa4jrjN7VxkS7QLnNPaaUCRVA7DF2FEN299JMIZV78RwUMdvGPaaUCRVvIdbmFyy_LSC..</t>
-  </si>
-  <si>
-    <t>土八热熔螺母</t>
-  </si>
-  <si>
-    <t>M2*2*3</t>
-  </si>
-  <si>
-    <t>https://detail.tmall.com/item.htm?id=809364062256&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.1e082e8dJs5w32&amp;pisk=gXH3sUq_1XPI37LT6AwBgw2VgsOTpJwSU4B8y8Uy_Pz6V6CpA7rrq4D-90z8E40oryFyRJHoSmiJAYKQLLqrkV2-vyU-S30KVTLBNJBPr2i2RDUJAY4zS2uuNHa8zz0-4XK9HKnIA8wzrEpvHARxRluhU9Pe45r8qhEefXJrg8wykUfOUW90F2yRXn5F_lz_qu7zz4Ja_uaa46yrzPPa0oQUU4uz7crQmM5PTTJabPZUzMzU4loamuEPTuurbhq77zyzT4oZi58U8YkKQFIyLOIbEgHYxW4qYymKjA-gw6i_SbhSBkc7GD55UTkgxWDag6oqqWhrcSMKvLX_pmcaQk0y3eyZ0fmYtvYcpzNoI2coJ3C7jbmrhJwc4pogKyVqKWs5nqoi4jFiBnJbKJzEwJiRmeniK2nII0IP_J2KsSD33K_UyfnmEuDWPd0mYjurZg-G_sW3LTZw2A55NWr_jrCZpr-WGr8dYhxGizNUfkzvjhf5NWr_jrKMjsm7TlZUk</t>
-  </si>
-  <si>
-    <t>3M同步轮</t>
-  </si>
-  <si>
-    <t>3M25齿 孔8 宽11</t>
-  </si>
-  <si>
-    <t>https://item.taobao.com/item.htm?spm=tbpc.boughtlist.suborder_itemtitle.1.1e082e8dJs5w32&amp;id=739009813395&amp;pisk=gS4g6qGIAlo6EvXKvyg14d0y43sLXVgbu-LxHqHVYvkCGhKO1ml4i-4YXSkxo-20nAnVCVU0K7NA1rCs7Zc4eJ0Y6AHYKs2TGEB1cVL2nRNPC5HA1rDqKRymc1Mx3x2YglCdyaF_1qgqnTQRyyS8CXrDuFlVgBltofrLbhEz1qgVnBLV2aV_CJRJHhlqT6cxMK843fJELvGvbxyqQDJEZbgqu-kaTBl-snRwuhlFtblX_xu2bBuEgjOwb-uVtWkIgqla3ql0aOkauPUFpI7wJQZholGijYPZI5eL83gkfJM35yaosoZu_nT2uycijyoyb7PmXoPSVPFOoegTZkuEs-7PQ2Pzx7ngSTYthm43Io2OMnG3mSzS54AV7W0iI0zifITuUWV42D4daagi7Arx5SdlBW4gB5a3MI-ESVEnqP0PPdkYv74mir6f-8Va4-rc4Exe4F0wlX5Y8ntjbXGneHztUssSUOdNt6xohclI_YChtntjbXGne6fHqSiZOfkR.</t>
-  </si>
-  <si>
-    <t>3M25齿 孔5 宽11</t>
-  </si>
-  <si>
-    <t>3M25齿 孔6 宽11</t>
-  </si>
-  <si>
-    <t>3M同步带</t>
-  </si>
-  <si>
-    <t>3M-长171-宽11</t>
-  </si>
-  <si>
-    <t>3M-长177-宽11</t>
-  </si>
-  <si>
-    <t>联轴器</t>
-  </si>
-  <si>
-    <t>外径28mm抱紧式联轴器 孔径8mm</t>
-  </si>
-  <si>
-    <t>https://buyertrade.taobao.com/trade/itemlist/list_bought_items.htm?spm=a21bo.jianhua/a.bought.1.5af92a89D0sxQv</t>
-  </si>
-  <si>
-    <t>限位开关</t>
-  </si>
-  <si>
-    <t>KW11-3Z-A</t>
-  </si>
-  <si>
-    <t>https://item.taobao.com/item.htm?spm=tbpc.boughtlist.suborder_itemtitle.1.12492e8dAwCxKM&amp;id=630808292950&amp;pisk=gprTs5D1d6fGaYZtKR7HilnkVyWnBw2aL5yWmjcMlWFLM8pgSqcmlmFzwqtc7c0xDWG3jf2ifxgbi7ai1PcDDoFU6hxmfSjxG8zF3fDgjKHbR5K0SRcgJKnaxPxms1oYh7mAZ_jlqRyZYm1lZXrvVsnSUxM6if9BRmDY-RTMFRyZ0j9HGa4QQKFhug9shj6KAxH6lmMjhJ6KHYhjcfgXOeMSOmiX5FTIdxktGjgbGeGI3AGXGqTsRMMohmT_GVsCpxlICmijMt5xOdGDDzfxdedv5g-pvkHtWjKmPneQq30xNtc90nltsVLgCXKXckUhggbj1aJngccanAFV4hoskPNtdmIvAcFaCogLm6vIyDGxPl0pFHg36x3Sc2pXcJnU8SMnVgOKLywgllP9HnMaju0xa2BX0qmQq4a76KWzdcMbg4rcahl_h8rzr0IvAc3f4Squ2GAyZbHD59BpuEusLy6btD2BkU3IpbXODE8q89kKZ9BpuEusLvhlBtL2u2WF.</t>
   </si>
 </sst>
 </file>
@@ -1209,7 +1212,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
@@ -1661,7 +1664,7 @@
         <v>59</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
       <c r="D25" s="5">
         <v>2</v>

</xml_diff>

<commit_message>
support mqtt control Signed-off-by: XG. <857439011@qq.com>
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12255"/>
+    <workbookView windowHeight="17680"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="65">
   <si>
     <t>序号</t>
   </si>
@@ -91,7 +91,7 @@
     <t>35步进电机</t>
   </si>
   <si>
-    <t>35-28 身长28</t>
+    <t>35-28</t>
   </si>
   <si>
     <t>https://item.taobao.com/item.htm?spm=tbpc.boughtlist.suborder_itemtitle.1.66912e8dUnU3HP&amp;id=723690490192&amp;pisk=gDY__fq9xR2sXf7YGGcURerI20_j5XurkS1vZIUaMNQOcrdwFszV0cfbl9O-sOomjKtBHpjNBtSVls9PKCzqsCljlIdRBZ-NQspehpqwQEW2LqOkFGzwMEPMxLR87FoGur_GoZHrU4ursCbckFlV2XygvsCSulEOkNbLUONZ24uysBNN6bRKzElbLUfaDrpAXMFdN9COHPIxOMCPMZUODPELp9XdkPCO6kEdg_EY6KUOv9C51tUYXZQKJs6d6opAMXOdKs_AHjh7Nsi1ICGNEZNoK5NWk9aYke1KnCA_XlXJI1gVLQWIeoYQrG6J69axE7mgGt6HyvoBtpx9Q6vjPv_pwH_O1K3849KB9FjytcHBNN6G2eISmrv55KsJWMNYzNABxw1pyjrlLe6wHFsKazsVJUSRWHonQi71NKLMCSaveBRySMYjFJBDb_bd1K3-dgJQzTi-koNCqr1CUXGQmoAsCJ8PUlBUwGCh1MlIORKcX6fCUXGQmojOt16EOXw9m</t>
@@ -100,7 +100,7 @@
     <t>35行星减速步进电机</t>
   </si>
   <si>
-    <t>35-26 身长28 减速比51</t>
+    <t>35-26 减速比51</t>
   </si>
   <si>
     <t>https://item.taobao.com/item.htm?spm=tbpc.boughtlist.suborder_itemtitle.1.66912e8dUnU3HP&amp;id=581976167345&amp;pisk=gHfasYTSa5FaVyt9I6OqYMaqExO9dIr7mstXoZbD5hxgHFNmgZ7klPEYW98ccMUYWC_D0iSBvjTbBohVYG_lCdsfCnYDxMbs1nN93i752iGb6OTmgM_vni1Vkj8coiU9cPeCWNdviuZ507_OWiVXrO5ZsDxhJUimIJ9iQW7_RuZ7NSyi-IraVisj60VHzUADSKcmKy8XocYcmKch-HLvocYmsyzevEHiIEYDteYy7IDiidVnxU8qncxMmX4eyHcMiIjDty8xMP7GoX8WIrep6Ni3RcKWqNxEibuRCdVh2xisf2T6L3vhejYCTFJwqNf15Aqy-61eFpgbqBbRdGYeaSlH_LWGbebL0b-GFaQWmd0iswdwYpxO8cDMzC-wE1vTNjO9n95e11qxew_ejLRCdJE6hCSNe3pgpkIV8hsc_pmaAn65R1vFqkGFDKWGbeAl4nmv-LYfMOom3dYp83aU8r_Z69ESIZXxHxpHwe-75FMxHdYp83aU8xHvKULeVPT1.</t>
@@ -205,7 +205,7 @@
     <t>外径28mm抱紧式联轴器 孔径8mm</t>
   </si>
   <si>
-    <t>https://buyertrade.taobao.com/trade/itemlist/list_bought_items.htm?spm=a21bo.jianhua/a.bought.1.5af92a89D0sxQv</t>
+    <t>https://detail.tmall.com/item.htm?id=667472622255&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.33e62e8dvP4q1L&amp;pisk=gzE7TiY8oQA5fD4tPDW2fTmJawiIFtSNvpMLIJKyp0n-RHez1v-E8aDBAjwOEb7hrWab9S0rwXuEAvNZi8-FE8WCAJetwDzravF4OSYzaklUgMwg14-zpkJuo5y94u7oYHioxDCN_GSNE8mnvsUq8PAlDYDCY33-e0mv_b9PWGSaE-9reOyAbkWHIHk2JHFKyqpxCjLpJ4FKknHnM3Hp2vdAhvcxvv3-pnHxdARpw3FpkEHtBQHKp23xkAksvXFKvtwxiviK9Wndh-hHdIMFPve5C1a_z_xZk8hXvHERxVGsBe-eYyM-Pke-G-y4cYgS6qbgTgr8gJEzqqbwSD245WaLMit7O8UT9brA6HGUSu2YcV9pY-ijORc-fpI8h0GSWoPlXHPThJUZloWOj0i-wyouLd1zhuNzEowepEnS4rg_VcIMwXz4CkMQx6jb18UT9ysPVhl1WMLBhVxIhfWfheY3F_O4bf8-gd3-nYINhtOX-4HmhfWfheYnyxD87t6XGef..</t>
   </si>
   <si>
     <t>限位开关</t>
@@ -218,6 +218,12 @@
   </si>
   <si>
     <t>KW11-3Z-B</t>
+  </si>
+  <si>
+    <t>M2*8</t>
+  </si>
+  <si>
+    <t>https://detail.tmall.com/item.htm?id=641493636015&amp;pisk=g0L8smfSGxDuTJ8RiQo0K7BtZlhDRmAygLR_-9XuAKpvpCFkqMXhAwpwBMan4ajdJK6DrTAlP6sBKdtlF3X3Jep2ez4hPp0ddC-qTTfkrWCBcLUHqQXkDWQyo34hEY7pOdbKIA0iSQRPuwMiIYohfz71s9ZQK_1flwfpmQZu1QRP89N0dcxXaWp22_F5O9GAl6C7Aws5OZNf36q5dp65c-1O_w_BdTabl1CGNy1QVjEf_6UQNT1Cho1F9u_CVpOjM6WfNw_IMbHdh763JhDl0vlnfrmsfECR29UHbyBMIPXCCiB0RAwdNgEkNtUQREKmLVmCFcPcLaXyt_pE7z75v39RGw3LlapyNesv-xVfXZ6dfUjY1rsDe6I1RiFQRIQ20p1c5VwAgnOkAUJ89y1yrFjdQihQ8MbXSGt6eWlwGa1BLG8nQzWWOC8wjN3LlaIC4KYMW42aIOC3VjhYYkS5gnGBnZAbvlIfMOc-JkrF0j5AIjhYYkS5gsBiwXEUYilV.&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.66912e8dUnU3HP</t>
   </si>
 </sst>
 </file>
@@ -1209,20 +1215,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="26.3666666666667" style="1" customWidth="1"/>
-    <col min="3" max="3" width="31.6333333333333" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.3636363636364" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.6363636363636" style="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="1"/>
-    <col min="5" max="5" width="47.0916666666667" style="1" customWidth="1"/>
-    <col min="6" max="6" width="66.0916666666667" style="2" customWidth="1"/>
+    <col min="5" max="5" width="47.0909090909091" style="1" customWidth="1"/>
+    <col min="6" max="6" width="66.0909090909091" style="2" customWidth="1"/>
     <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -1350,7 +1356,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="5"/>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="7" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1440,7 +1446,7 @@
         <v>32</v>
       </c>
       <c r="E12" s="5"/>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="7" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1634,7 +1640,7 @@
         <v>5</v>
       </c>
       <c r="E23" s="5"/>
-      <c r="F23" s="8" t="s">
+      <c r="F23" s="7" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1672,6 +1678,24 @@
       <c r="E25" s="5"/>
       <c r="F25" s="7" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="26" ht="15" customHeight="1" spans="1:6">
+      <c r="A26" s="10">
+        <v>27</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="10">
+        <v>10</v>
+      </c>
+      <c r="E26" s="10"/>
+      <c r="F26" s="8" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1679,16 +1703,16 @@
     <hyperlink ref="F2" r:id="rId1" display="https://item.taobao.com/item.htm?spm=tbpc.boughtlist.suborder_itemtitle.1.722b2e8dO34cYk&amp;id=526104907428&amp;pisk=gLmasf254hKwx3VTSDZVTX6ZUrZTSoRWimNbnxD0C5VMkRtc0xkuhddvB2ymGXpvBlM0gjlQ9iwXWIIqTfMo5PGj5S20tXD1fStTujkSwjsXXVwc0XMYojiqHiymnjpTGdLIBAEYmQOSg3MtB5hx0ymaiHjnp-ecSeaG7Hk6dQOWVn8GKoRwNjGbk7-3U8q0IrjcxpyzEZq0oRDHL-2fsZjiipJUh8yciS40KM28Iobgo-qnK8eai1V0o9vUHWV0moc0xpyxGgDinMy7SKLLnD_hSgEUZAVFmgW8mPjZdZsGjX2g7mDgTp9IYRzaZyL-GhiiOxmsXyL5yoHIzjumtHSZgA0oi5iHZiPjycHnYzWccvrUgYFg4txiLlParDG9qiGoLx078D9k2lrgsqZthTRsLclsBDkfnwqaf2zrbuxRsSgIUmyqDIKEaA0oiqSz4se3r-ix7sb4SJeUNpJehAStJQ_inqQAkyq8L79_CZQY7jeUNp6CkZU13JPWdmf.." tooltip="https://item.taobao.com/item.htm?spm=tbpc.boughtlist.suborder_itemtitle.1.722b2e8dO34cYk&amp;id=526104907428&amp;pisk=gLmasf254hKwx3VTSDZVTX6ZUrZTSoRWimNbnxD0C5VMkRtc0xkuhddvB2ymGXpvBlM0gjlQ9iwXWIIqTfMo5PGj5S20tXD1fStTujkSwjsXXVwc0XMYojiqHiymnjpTGdLIBAEYmQOSg3MtB"/>
     <hyperlink ref="F3" r:id="rId1" display="https://item.taobao.com/item.htm?spm=tbpc.boughtlist.suborder_itemtitle.1.722b2e8dO34cYk&amp;id=526104907428&amp;pisk=gLmasf254hKwx3VTSDZVTX6ZUrZTSoRWimNbnxD0C5VMkRtc0xkuhddvB2ymGXpvBlM0gjlQ9iwXWIIqTfMo5PGj5S20tXD1fStTujkSwjsXXVwc0XMYojiqHiymnjpTGdLIBAEYmQOSg3MtB5hx0ymaiHjnp-ecSeaG7Hk6dQOWVn8GKoRwNjGbk7-3U8q0IrjcxpyzEZq0oRDHL-2fsZjiipJUh8yciS40KM28Iobgo-qnK8eai1V0o9vUHWV0moc0xpyxGgDinMy7SKLLnD_hSgEUZAVFmgW8mPjZdZsGjX2g7mDgTp9IYRzaZyL-GhiiOxmsXyL5yoHIzjumtHSZgA0oi5iHZiPjycHnYzWccvrUgYFg4txiLlParDG9qiGoLx078D9k2lrgsqZthTRsLclsBDkfnwqaf2zrbuxRsSgIUmyqDIKEaA0oiqSz4se3r-ix7sb4SJeUNpJehAStJQ_inqQAkyq8L79_CZQY7jeUNp6CkZU13JPWdmf.."/>
     <hyperlink ref="F4" r:id="rId2" display="https://item.taobao.com/item.htm?id=681246792404&amp;pisk=gLHTsSq6AeYGW5DTxcRhoGUJj_KnXBmZYVo5nr4GG23Kk0IisS40G-3ryS6D_RVYH2anIPmgCoNjo4Gg5f4cHx3EWOX0CqvYl0le0PqiIiEjOVBmsc4i9ieZKfX0SFyxc42vrUvkEcoaL-TkrFR0NOy7Xr_1oosIA-qxtc1GVcoa3rshlQcIbi3EgBj_crtLdoE1h-N_hJ_Q8of_lqa_OwZ84-wjlP6CduEuftZf1HCQboEfho66dWZzctwbhqiBvozQf-wjGP8YRGacHbYgTE-cbQWRevET6rB0ytEsLTVgPPUChUwUXazSfyBfhPv2b9iKjFBrxRkEyu0MdO3-fbgjN29dBWlsvxFr3IXif-UTZANOfFPLMPhICWIfhcoE9qcxWFCa5f0LakNCDLrnryiZCXKVRcguWRZQtLt-ASGnQ7kMROeSac2iG29dB4srmYDJIa7uyof6vHCVg5ZEOng3KD1AwWZLrhpAgsPeYkUkvHCVg5ZUvzx9Ds54TH5..&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.66912e8dUnU3HP"/>
-    <hyperlink ref="F5" r:id="rId3" display="https://item.taobao.com/item.htm?id=673302946671&amp;pisk=g3S7660Robc5PiKKdU2qciubWPtIR-ravv9dI9nrp3KJRDBP1poe8zvIAI6TEQz3r6_f9sYywB8eAp1wiToUETyQA9B9wH7yapCVOs0PaMRFgk6G1UoPpMklo1Wt4gzkYDtkxHFa_lraETxHvgyeW-loMpv7YDp-23xx_QMzWlrNEtMyeRWYbMyI0Mp-JDCpyEHvCIhppHCpkmpHM0pK2phYhIAx24pJpqKvIdkJvpnJMIpHLYnppphvDIvpvBCpv-tviphvdA9QPQX7UCxIISqUc6OjvDIXHWxGFynWQMpSXCXXG5HNccYW6Tdjv5DgrvOBiGF4ltfcy_JcOlNXDOQX2L1LXVRAltIk7t48GOtWZFIv5ymh131BWgLjpc-lhZxXHGeESISXa6IWkRo68nIwW3Q4o78eVd1dq_MIv1BVQgYcA5GvtaJMDL1LXSsrAcR_Wk3IhFmBhCybh20hF7GVbCuJgALJnLT4h-GR-UpDhCybh20HyKvWg-wjwwf..&amp;skuId=5032954871244&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.66912e8dUnU3HP"/>
+    <hyperlink ref="F5" r:id="rId3" display="https://item.taobao.com/item.htm?id=673302946671&amp;pisk=g3S7660Robc5PiKKdU2qciubWPtIR-ravv9dI9nrp3KJRDBP1poe8zvIAI6TEQz3r6_f9sYywB8eAp1wiToUETyQA9B9wH7yapCVOs0PaMRFgk6G1UoPpMklo1Wt4gzkYDtkxHFa_lraETxHvgyeW-loMpv7YDp-23xx_QMzWlrNEtMyeRWYbMyI0Mp-JDCpyEHvCIhppHCpkmpHM0pK2phYhIAx24pJpqKvIdkJvpnJMIpHLYnppphvDIvpvBCpv-tviphvdA9QPQX7UCxIISqUc6OjvDIXHWxGFynWQMpSXCXXG5HNccYW6Tdjv5DgrvOBiGF4ltfcy_JcOlNXDOQX2L1LXVRAltIk7t48GOtWZFIv5ymh131BWgLjpc-lhZxXHGeESISXa6IWkRo68nIwW3Q4o78eVd1dq_MIv1BVQgYcA5GvtaJMDL1LXSsrAcR_Wk3IhFmBhCybh20hF7GVbCuJgALJnLT4h-GR-UpDhCybh20HyKvWg-wjwwf..&amp;skuId=5032954871244&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.66912e8dUnU3HP" tooltip="https://item.taobao.com/item.htm?id=673302946671&amp;pisk=g3S7660Robc5PiKKdU2qciubWPtIR-ravv9dI9nrp3KJRDBP1poe8zvIAI6TEQz3r6_f9sYywB8eAp1wiToUETyQA9B9wH7yapCVOs0PaMRFgk6G1UoPpMklo1Wt4gzkYDtkxHFa_lraETxHvgyeW-loMpv7YDp-23xx_QMzWlrNEtMyeRWYbMyI0Mp-JDCpyEHvCIhpp"/>
     <hyperlink ref="F6" r:id="rId4" display="https://item.taobao.com/item.htm?id=21034340111&amp;pisk=gDPL_i0C5Gj3ZzNKSyWMqenA-KQMpO4U7kzXZ0mHFlET2rL3KYmoFbE4DYOlLXD-wligtD4nO4M7qownAJmkw7EavBAoOuf-VryNzD03tU37CkduKym3BUhUsJAoxMl8PocRmifciyzE_bscmMWohBljkeOBqYts1b08Iy9HlyzEa0TMVt2_8UEanT8SP0_t143BFbMINhMsb4vIVuiIChgxubG7VDO61q3mRQgWdNHsr4OBNDi75fgoybgIVuG_5cuSN2ZSNjhP2cTIqQecxASPrCT9xHVtJvnJZuA-LROmwmOiYBAnvWMpKyi9NQNTIg5cFD62S0lnYz0L4sREOYeQvVGRwCGLYyNSB7jM5xhs2xNnBEOsIk3-hbM9PQat_RrSSj1XXVy_-8NUvUdS8WVmemkOPQko1SDbhkLPuPGIPuk4ZiREAza4g-cAwCGKFgr0iSCH0nmxrp_OWLJrdVy1Plcg5LpxCVncJ_pyUA7ZWmbOWLJrdVutmwQJULkN7&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.66912e8dUnU3HP&amp;sku_properties=1627207%3A33214301305"/>
     <hyperlink ref="F7" r:id="rId5" display="https://item.taobao.com/item.htm?spm=tbpc.boughtlist.suborder_itemtitle.1.66912e8dUnU3HP&amp;id=723690490192&amp;pisk=gDY__fq9xR2sXf7YGGcURerI20_j5XurkS1vZIUaMNQOcrdwFszV0cfbl9O-sOomjKtBHpjNBtSVls9PKCzqsCljlIdRBZ-NQspehpqwQEW2LqOkFGzwMEPMxLR87FoGur_GoZHrU4ursCbckFlV2XygvsCSulEOkNbLUONZ24uysBNN6bRKzElbLUfaDrpAXMFdN9COHPIxOMCPMZUODPELp9XdkPCO6kEdg_EY6KUOv9C51tUYXZQKJs6d6opAMXOdKs_AHjh7Nsi1ICGNEZNoK5NWk9aYke1KnCA_XlXJI1gVLQWIeoYQrG6J69axE7mgGt6HyvoBtpx9Q6vjPv_pwH_O1K3849KB9FjytcHBNN6G2eISmrv55KsJWMNYzNABxw1pyjrlLe6wHFsKazsVJUSRWHonQi71NKLMCSaveBRySMYjFJBDb_bd1K3-dgJQzTi-koNCqr1CUXGQmoAsCJ8PUlBUwGCh1MlIORKcX6fCUXGQmojOt16EOXw9m"/>
     <hyperlink ref="F8" r:id="rId6" display="https://item.taobao.com/item.htm?spm=tbpc.boughtlist.suborder_itemtitle.1.66912e8dUnU3HP&amp;id=581976167345&amp;pisk=gHfasYTSa5FaVyt9I6OqYMaqExO9dIr7mstXoZbD5hxgHFNmgZ7klPEYW98ccMUYWC_D0iSBvjTbBohVYG_lCdsfCnYDxMbs1nN93i752iGb6OTmgM_vni1Vkj8coiU9cPeCWNdviuZ507_OWiVXrO5ZsDxhJUimIJ9iQW7_RuZ7NSyi-IraVisj60VHzUADSKcmKy8XocYcmKch-HLvocYmsyzevEHiIEYDteYy7IDiidVnxU8qncxMmX4eyHcMiIjDty8xMP7GoX8WIrep6Ni3RcKWqNxEibuRCdVh2xisf2T6L3vhejYCTFJwqNf15Aqy-61eFpgbqBbRdGYeaSlH_LWGbebL0b-GFaQWmd0iswdwYpxO8cDMzC-wE1vTNjO9n95e11qxew_ejLRCdJE6hCSNe3pgpkIV8hsc_pmaAn65R1vFqkGFDKWGbeAl4nmv-LYfMOom3dYp83aU8r_Z69ESIZXxHxpHwe-75FMxHdYp83aU8xHvKULeVPT1."/>
     <hyperlink ref="F9" r:id="rId7" display="https://item.taobao.com/item.htm?spm=tbpc.boughtlist.suborder_itemtitle.1.66912e8dUnU3HP&amp;id=736578173538&amp;pisk=gXtT_QXsdXcgEs-OKdu3iRC-IzHnX2vwLCJ7msfglBdpMLeMSZfclidywZZm7GbADB1Hj1vGft_XiQTG1Ff0Dnde6lqcfImAGL8E31XMj-BXRCEDSdfMJ-IwxFqcsfSvhQjxZbmoqdJNYiGoZfucPlS5CrabiZ6CRiXv-dagFdJN0sw3G4YBQ-dezz2fhsMdAtB_li_1cW_CTt41GI11RW6RUisXG1ZQATBlCo6b5vFChT4_1o__O66l3Ssf1IsCO6WfcOOfcj4iM6w1ioLoswlqnfFI0m-dBNCYmhrAxBqln_aF6oEA6vb1N0fLcotdBp03SuE-o_TPsafHODqODp6vwTdTOXIXph-RRhGUDwRAOwt18-ZWeCxOAhT8ho9dX6RcdCPt9_twd3SC-0MJdHRMQHp0hm6HZ69wfinSUGI11MBemXr1MeTXjNS41fIXptszi3x-j7Plwt4spvU4uN6eRxOhxpaYyw6dZAnYur7EL9CopvU4uN6Fp_DtHrzV8v5.."/>
     <hyperlink ref="F11" r:id="rId8" display="https://detail.tmall.com/item.htm?id=616787169746&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.66912e8dUnU3HP&amp;pisk=g2Dgsk6FFfP6eYYL9vw6aaGV4uAL-Rwj3qBYk-U2TyzBc1C9fSrqmqDx6mzYnq0moPF25RHm-0ivfxK_QKqqy22xXPUx-n0tctL6GRBVoViy5cUvfx44-Vu0GhaYur0x0fKpeLnsf-w4nUpJerVXm80GgOrw09r_4HEwAfJqa-w2yEfd359uhVyAlb1NTkzQmo740qyUToq43ora3H4Umu1V7qu2xyr8qs54_r5eLyZ8bsWN3wyUqlbN3ou48HqY8ry4_qoEiRW4rxkILeILHtKsngN3j54rbPoTBv5Qv1Ma-R2sIlmHxc43vkH3j54zOQgvBAuK0AH_OQC7hDhoojueKO0mbbu4Wv8PnrhSCDk3ZiWxxJ4mVPyl0do3IPVrpV9PH4on0bFnp3J7IRzZMRiAqFnnIVnsKmIVTR2tt7DgUL_akXnonoDXlp0obbuqigyNT_r05tZeDv5fG5rQxzCEBz-Xhtj4EHxhNCNaAlLJxHffG5rQxzKHx____kZ9y"/>
     <hyperlink ref="F10" r:id="rId9" display="https://item.taobao.com/item.htm?id=736578173538&amp;pisk=gXtT_QXsdXcgEs-OKdu3iRC-IzHnX2vwLCJ7msfglBdpMLeMSZfclidywZZm7GbADB1Hj1vGft_XiQTG1Ff0Dnde6lqcfImAGL8E31XMj-BXRCEDSdfMJ-IwxFqcsfSvhQjxZbmoqdJNYiGoZfucPlS5CrabiZ6CRiXv-dagFdJN0sw3G4YBQ-dezz2fhsMdAtB_li_1cW_CTt41GI11RW6RUisXG1ZQATBlCo6b5vFChT4_1o__O66l3Ssf1IsCO6WfcOOfcj4iM6w1ioLoswlqnfFI0m-dBNCYmhrAxBqln_aF6oEA6vb1N0fLcotdBp03SuE-o_TPsafHODqODp6vwTdTOXIXph-RRhGUDwRAOwt18-ZWeCxOAhT8ho9dX6RcdCPt9_twd3SC-0MJdHRMQHp0hm6HZ69wfinSUGI11MBemXr1MeTXjNS41fIXptszi3x-j7Plwt4spvU4uN6eRxOhxpaYyw6dZAnYur7EL9CopvU4uN6Fp_DtHrzV8v5..&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.66912e8dUnU3HP"/>
-    <hyperlink ref="F12" r:id="rId10" display="https://detail.tmall.com/item.htm?id=641493636015&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.66912e8dUnU3HP&amp;pisk=g0L8smfSGxDuTJ8RiQo0K7BtZlhDRmAygLR_-9XuAKpvpCFkqMXhAwpwBMan4ajdJK6DrTAlP6sBKdtlF3X3Jep2ez4hPp0ddC-qTTfkrWCBcLUHqQXkDWQyo34hEY7pOdbKIA0iSQRPuwMiIYohfz71s9ZQK_1flwfpmQZu1QRP89N0dcxXaWp22_F5O9GAl6C7Aws5OZNf36q5dp65c-1O_w_BdTabl1CGNy1QVjEf_6UQNT1Cho1F9u_CVpOjM6WfNw_IMbHdh763JhDl0vlnfrmsfECR29UHbyBMIPXCCiB0RAwdNgEkNtUQREKmLVmCFcPcLaXyt_pE7z75v39RGw3LlapyNesv-xVfXZ6dfUjY1rsDe6I1RiFQRIQ20p1c5VwAgnOkAUJ89y1yrFjdQihQ8MbXSGt6eWlwGa1BLG8nQzWWOC8wjN3LlaIC4KYMW42aIOC3VjhYYkS5gnGBnZAbvlIfMOc-JkrF0j5AIjhYYkS5gsBiwXEUYilV."/>
+    <hyperlink ref="F12" r:id="rId10" display="https://detail.tmall.com/item.htm?id=641493636015&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.66912e8dUnU3HP&amp;pisk=g0L8smfSGxDuTJ8RiQo0K7BtZlhDRmAygLR_-9XuAKpvpCFkqMXhAwpwBMan4ajdJK6DrTAlP6sBKdtlF3X3Jep2ez4hPp0ddC-qTTfkrWCBcLUHqQXkDWQyo34hEY7pOdbKIA0iSQRPuwMiIYohfz71s9ZQK_1flwfpmQZu1QRP89N0dcxXaWp22_F5O9GAl6C7Aws5OZNf36q5dp65c-1O_w_BdTabl1CGNy1QVjEf_6UQNT1Cho1F9u_CVpOjM6WfNw_IMbHdh763JhDl0vlnfrmsfECR29UHbyBMIPXCCiB0RAwdNgEkNtUQREKmLVmCFcPcLaXyt_pE7z75v39RGw3LlapyNesv-xVfXZ6dfUjY1rsDe6I1RiFQRIQ20p1c5VwAgnOkAUJ89y1yrFjdQihQ8MbXSGt6eWlwGa1BLG8nQzWWOC8wjN3LlaIC4KYMW42aIOC3VjhYYkS5gnGBnZAbvlIfMOc-JkrF0j5AIjhYYkS5gsBiwXEUYilV." tooltip="https://detail.tmall.com/item.htm?id=641493636015&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.66912e8dUnU3HP&amp;pisk=g0L8smfSGxDuTJ8RiQo0K7BtZlhDRmAygLR_-9XuAKpvpCFkqMXhAwpwBMan4ajdJK6DrTAlP6sBKdtlF3X3Jep2ez4hPp0ddC-qTTfkrWCBcLUHqQXkDWQyo34hEY7pOdbKIA0iSQRPuwMi"/>
     <hyperlink ref="F15" r:id="rId11" display="https://detail.tmall.com/item.htm?detail_redpacket_pop=true&amp;id=549640610734&amp;ltk2=1751972028937ji8m1jp7ssaci3uz6zdys&amp;ns=1&amp;priceTId=undefined&amp;query=m5%E8%9E%BA%E6%AF%8D&amp;skuId=5618615008389&amp;spm=a21n57.1.hoverItem.1&amp;utparam=%7B%22aplus_abtest%22%3A%2203691c8cc532103ef1eb26baed91686a%22%7D&amp;xxc=ad_ztc"/>
-    <hyperlink ref="F23" r:id="rId12" display="https://buyertrade.taobao.com/trade/itemlist/list_bought_items.htm?spm=a21bo.jianhua/a.bought.1.5af92a89D0sxQv"/>
+    <hyperlink ref="F23" r:id="rId12" display="https://detail.tmall.com/item.htm?id=667472622255&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.33e62e8dvP4q1L&amp;pisk=gzE7TiY8oQA5fD4tPDW2fTmJawiIFtSNvpMLIJKyp0n-RHez1v-E8aDBAjwOEb7hrWab9S0rwXuEAvNZi8-FE8WCAJetwDzravF4OSYzaklUgMwg14-zpkJuo5y94u7oYHioxDCN_GSNE8mnvsUq8PAlDYDCY33-e0mv_b9PWGSaE-9reOyAbkWHIHk2JHFKyqpxCjLpJ4FKknHnM3Hp2vdAhvcxvv3-pnHxdARpw3FpkEHtBQHKp23xkAksvXFKvtwxiviK9Wndh-hHdIMFPve5C1a_z_xZk8hXvHERxVGsBe-eYyM-Pke-G-y4cYgS6qbgTgr8gJEzqqbwSD245WaLMit7O8UT9brA6HGUSu2YcV9pY-ijORc-fpI8h0GSWoPlXHPThJUZloWOj0i-wyouLd1zhuNzEowepEnS4rg_VcIMwXz4CkMQx6jb18UT9ysPVhl1WMLBhVxIhfWfheY3F_O4bf8-gd3-nYINhtOX-4HmhfWfheYnyxD87t6XGef.." tooltip="https://detail.tmall.com/item.htm?id=667472622255&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.33e62e8dvP4q1L&amp;pisk=gzE7TiY8oQA5fD4tPDW2fTmJawiIFtSNvpMLIJKyp0n-RHez1v-E8aDBAjwOEb7hrWab9S0rwXuEAvNZi8-FE8WCAJetwDzravF4OSYzaklUgMwg14-zpkJuo5y94u7oYHioxDCN_GSNE8mn"/>
     <hyperlink ref="F16" r:id="rId13" display="https://detail.tmall.com/item.htm?id=549640610734&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.1e082e8dJs5w32&amp;pisk=gHo3_1w_52zQ_gATWcZBu6qVuZTtRkZS4bI8wuFy75P6FwQpdzyrEbm-JYP8qbcoZWUyOknosxMJd0pQY32rMfq-pWF-sLcKFgdBPkIPZXM2OvFJd0VzsXluPpN8a7c-U2p9DnHIduZzZIKvDc8xORlh8WPyUPy7UdeeC2-ruuZyMQbO4yt0VXrRB9_P7RP_E85zab-a78NaUwrra5za3-CU4blz_AyQn97P8g-aQ5wc49yzaA7ae85FY7lrQd28EuPrayJiQjf2TWorvcROUHSOhzRsYJ43gvPnpAmwlP_Ip5mxVcynPJMFPgSrjJ4nbr7E3Y4KzxajvvKlfkHm7lynanRUbxuiHymHiMF7rccnrXpRPR0oUmZQmT-EIkV3uD4CFicqIYuYScp2ckqUT4EIetAKIDcKdcDRUNr3vV4mxo-fT73tn02oVQtiivuqa4jrjN7VxkS7QLnNPaaUCRVA7DF2FEN299JMIZV78RwUMdvGPaaUCRVvIdbmFyy_LSC.."/>
     <hyperlink ref="F17" r:id="rId14" display="https://detail.tmall.com/item.htm?id=809364062256&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.1e082e8dJs5w32&amp;pisk=gXH3sUq_1XPI37LT6AwBgw2VgsOTpJwSU4B8y8Uy_Pz6V6CpA7rrq4D-90z8E40oryFyRJHoSmiJAYKQLLqrkV2-vyU-S30KVTLBNJBPr2i2RDUJAY4zS2uuNHa8zz0-4XK9HKnIA8wzrEpvHARxRluhU9Pe45r8qhEefXJrg8wykUfOUW90F2yRXn5F_lz_qu7zz4Ja_uaa46yrzPPa0oQUU4uz7crQmM5PTTJabPZUzMzU4loamuEPTuurbhq77zyzT4oZi58U8YkKQFIyLOIbEgHYxW4qYymKjA-gw6i_SbhSBkc7GD55UTkgxWDag6oqqWhrcSMKvLX_pmcaQk0y3eyZ0fmYtvYcpzNoI2coJ3C7jbmrhJwc4pogKyVqKWs5nqoi4jFiBnJbKJzEwJiRmeniK2nII0IP_J2KsSD33K_UyfnmEuDWPd0mYjurZg-G_sW3LTZw2A55NWr_jrCZpr-WGr8dYhxGizNUfkzvjhf5NWr_jrKMjsm7TlZUk"/>
     <hyperlink ref="F18" r:id="rId15" display="https://item.taobao.com/item.htm?spm=tbpc.boughtlist.suborder_itemtitle.1.1e082e8dJs5w32&amp;id=739009813395&amp;pisk=gS4g6qGIAlo6EvXKvyg14d0y43sLXVgbu-LxHqHVYvkCGhKO1ml4i-4YXSkxo-20nAnVCVU0K7NA1rCs7Zc4eJ0Y6AHYKs2TGEB1cVL2nRNPC5HA1rDqKRymc1Mx3x2YglCdyaF_1qgqnTQRyyS8CXrDuFlVgBltofrLbhEz1qgVnBLV2aV_CJRJHhlqT6cxMK843fJELvGvbxyqQDJEZbgqu-kaTBl-snRwuhlFtblX_xu2bBuEgjOwb-uVtWkIgqla3ql0aOkauPUFpI7wJQZholGijYPZI5eL83gkfJM35yaosoZu_nT2uycijyoyb7PmXoPSVPFOoegTZkuEs-7PQ2Pzx7ngSTYthm43Io2OMnG3mSzS54AV7W0iI0zifITuUWV42D4daagi7Arx5SdlBW4gB5a3MI-ESVEnqP0PPdkYv74mir6f-8Va4-rc4Exe4F0wlX5Y8ntjbXGneHztUssSUOdNt6xohclI_YChtntjbXGne6fHqSiZOfkR."/>
@@ -1698,6 +1722,7 @@
     <hyperlink ref="F13" r:id="rId16" display="https://detail.tmall.com/item.htm?id=40189700729&amp;pisk=gJG_s6cDkGj6j-PAlRYFOvo2Z7Vb5eRyMZaxrqCNk5FThs3ZVr543d4fGkgJSlJDImMIDD2aXoy4GrizxV52SV8XGq38XSkabrnEcDXZbjrqYIgoVR5Zkj7iK0uR_fJggsNgiSKy4QRr7VV0MGdi8PsgJzU6grETD5Vd4l_weQRrS2_aWUupaj8X6P41HsnYBJQLrkUTkOU9RJUzkSCTH1BdvkqLMreYMyBLkr6OHRnYJ2U4WNITMSILpPrLDSFxD2LQlkExMxvQJdZE5Fr6zQUBBBM3AsCxOyt08V_1dol45YqSWVvkEE4_Cu3TAhCJWBwKo-GcoswZWYm0ycI9fS3QP0aSfK70fv3r_x36O3FZsVH8HbKcH0Nsc8hTdZCjS5r3OyhJuTqEOlox1JLPN-PKa8FtLpxa35aSDfm1lsn-84lgKjt5voDarWUsDQKC4zCzVDHGhwwlGyZyRe6cnVt1Ybz4fVUbBy4hzeTCUt2T-yZyRe6cnRU3-Q8BRTWc.&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.66b22e8dWKj7Gf"/>
     <hyperlink ref="F24" r:id="rId17" display="https://item.taobao.com/item.htm?spm=tbpc.boughtlist.suborder_itemtitle.1.12492e8dAwCxKM&amp;id=630808292950&amp;pisk=gprTs5D1d6fGaYZtKR7HilnkVyWnBw2aL5yWmjcMlWFLM8pgSqcmlmFzwqtc7c0xDWG3jf2ifxgbi7ai1PcDDoFU6hxmfSjxG8zF3fDgjKHbR5K0SRcgJKnaxPxms1oYh7mAZ_jlqRyZYm1lZXrvVsnSUxM6if9BRmDY-RTMFRyZ0j9HGa4QQKFhug9shj6KAxH6lmMjhJ6KHYhjcfgXOeMSOmiX5FTIdxktGjgbGeGI3AGXGqTsRMMohmT_GVsCpxlICmijMt5xOdGDDzfxdedv5g-pvkHtWjKmPneQq30xNtc90nltsVLgCXKXckUhggbj1aJngccanAFV4hoskPNtdmIvAcFaCogLm6vIyDGxPl0pFHg36x3Sc2pXcJnU8SMnVgOKLywgllP9HnMaju0xa2BX0qmQq4a76KWzdcMbg4rcahl_h8rzr0IvAc3f4Squ2GAyZbHD59BpuEusLy6btD2BkU3IpbXODE8q89kKZ9BpuEusLvhlBtL2u2WF." tooltip="https://item.taobao.com/item.htm?spm=tbpc.boughtlist.suborder_itemtitle.1.12492e8dAwCxKM&amp;id=630808292950&amp;pisk=gprTs5D1d6fGaYZtKR7HilnkVyWnBw2aL5yWmjcMlWFLM8pgSqcmlmFzwqtc7c0xDWG3jf2ifxgbi7ai1PcDDoFU6hxmfSjxG8zF3fDgjKHbR5K0SRcgJKnaxPxms1oYh7mAZ_jlqRyZYm1lZ"/>
     <hyperlink ref="F25" r:id="rId17" display="https://item.taobao.com/item.htm?spm=tbpc.boughtlist.suborder_itemtitle.1.12492e8dAwCxKM&amp;id=630808292950&amp;pisk=gprTs5D1d6fGaYZtKR7HilnkVyWnBw2aL5yWmjcMlWFLM8pgSqcmlmFzwqtc7c0xDWG3jf2ifxgbi7ai1PcDDoFU6hxmfSjxG8zF3fDgjKHbR5K0SRcgJKnaxPxms1oYh7mAZ_jlqRyZYm1lZXrvVsnSUxM6if9BRmDY-RTMFRyZ0j9HGa4QQKFhug9shj6KAxH6lmMjhJ6KHYhjcfgXOeMSOmiX5FTIdxktGjgbGeGI3AGXGqTsRMMohmT_GVsCpxlICmijMt5xOdGDDzfxdedv5g-pvkHtWjKmPneQq30xNtc90nltsVLgCXKXckUhggbj1aJngccanAFV4hoskPNtdmIvAcFaCogLm6vIyDGxPl0pFHg36x3Sc2pXcJnU8SMnVgOKLywgllP9HnMaju0xa2BX0qmQq4a76KWzdcMbg4rcahl_h8rzr0IvAc3f4Squ2GAyZbHD59BpuEusLy6btD2BkU3IpbXODE8q89kKZ9BpuEusLvhlBtL2u2WF."/>
+    <hyperlink ref="F26" r:id="rId18" display="https://detail.tmall.com/item.htm?id=641493636015&amp;pisk=g0L8smfSGxDuTJ8RiQo0K7BtZlhDRmAygLR_-9XuAKpvpCFkqMXhAwpwBMan4ajdJK6DrTAlP6sBKdtlF3X3Jep2ez4hPp0ddC-qTTfkrWCBcLUHqQXkDWQyo34hEY7pOdbKIA0iSQRPuwMiIYohfz71s9ZQK_1flwfpmQZu1QRP89N0dcxXaWp22_F5O9GAl6C7Aws5OZNf36q5dp65c-1O_w_BdTabl1CGNy1QVjEf_6UQNT1Cho1F9u_CVpOjM6WfNw_IMbHdh763JhDl0vlnfrmsfECR29UHbyBMIPXCCiB0RAwdNgEkNtUQREKmLVmCFcPcLaXyt_pE7z75v39RGw3LlapyNesv-xVfXZ6dfUjY1rsDe6I1RiFQRIQ20p1c5VwAgnOkAUJ89y1yrFjdQihQ8MbXSGt6eWlwGa1BLG8nQzWWOC8wjN3LlaIC4KYMW42aIOC3VjhYYkS5gnGBnZAbvlIfMOc-JkrF0j5AIjhYYkS5gsBiwXEUYilV.&amp;spm=tbpc.boughtlist.suborder_itemtitle.1.66912e8dUnU3HP"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1714,7 +1739,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1731,7 +1756,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>